<commit_message>
update 11 Dec 23 - from IIMV onedrive
</commit_message>
<xml_diff>
--- a/Capex/raw_data/Book1.xlsx
+++ b/Capex/raw_data/Book1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26903"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -180,7 +180,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -230,7 +230,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -548,12 +548,12 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="98.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18.95">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,12 +567,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.95">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.95">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -598,7 +598,7 @@
         <v>0.45985401459854014</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.95">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -624,7 +624,7 @@
         <v>0.53379629629629632</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.95">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -650,7 +650,7 @@
         <v>0.67114093959731547</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.95">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -676,7 +676,7 @@
         <v>0.60067681895093061</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.95">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -702,7 +702,7 @@
         <v>0.80989065606361832</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18.95">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -728,7 +728,7 @@
         <v>0.5444444444444444</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18.95">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -754,7 +754,7 @@
         <v>0.79547790339157243</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="18.95">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -780,7 +780,7 @@
         <v>0.27906976744186046</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="18.95">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -806,7 +806,7 @@
         <v>0.94117647058823528</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="18.95">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -832,7 +832,7 @@
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="18.95">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -858,7 +858,7 @@
         <v>0.8694187026116259</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="18.95">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -884,7 +884,7 @@
         <v>0.54827280779450838</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="18.95">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -910,7 +910,7 @@
         <v>0.62662807525325614</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="18.95">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -936,7 +936,7 @@
         <v>0.65034280117531829</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="18.95">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -962,7 +962,7 @@
         <v>0.76380368098159512</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="18.95">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -988,7 +988,7 @@
         <v>0.72879776328052193</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="18.95">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>0.53838451268357812</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="18.95">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>0.61651131824234351</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="18.95">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>0.59420289855072461</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="18.95">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="18.95">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="18.95">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>0.80483525053616689</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="18.95">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>0.65530375166634924</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="18.95">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>0.70671378091872794</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="18.95">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>0.6992481203007519</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="18.95">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>0.82692307692307687</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="18.95">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>0.56721915285451197</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="18.95">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>0.75625823451910412</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="18.95">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>0.70161290322580649</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="18.95">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>0.78778337531486142</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="18.95">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>0.60317460317460314</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="18.95">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>0.5731225296442688</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="18.95">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>0.54430005906674539</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="18.95">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>0.13311688311688311</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="18.95">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>0.58809276566285917</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="18.95">
       <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>0.63217031342400942</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="18.95">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>0.73456790123456794</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="18.95">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>0.95454545454545459</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="18.95">
       <c r="A41" s="1" t="s">
         <v>43</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>0.54961197339246115</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="18.95">
       <c r="A42" s="1" t="s">
         <v>44</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>0.61367837338262476</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="18.95">
       <c r="A43" s="1" t="s">
         <v>45</v>
       </c>

</xml_diff>